<commit_message>
Still some issues but mostly complete
</commit_message>
<xml_diff>
--- a/new_data/SO_Line_Items_12_Orders_Revised.xlsx
+++ b/new_data/SO_Line_Items_12_Orders_Revised.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\source\bundle-optimization\new_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\source\bundle-optimization-new\new_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E74784-C1C0-4677-8889-8E28C62D45D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ECDA2C-CE40-4C14-B99B-82868A5398ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SKU_Quantities" sheetId="1" r:id="rId1"/>
     <sheet name="SO_Input" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SKU_Quantities!$A$1:$C$122</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -810,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="A1:D122"/>
     </sheetView>
   </sheetViews>
@@ -2181,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B55D905-81B1-4C30-9105-ACE57A38A51C}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished tool; works as intended with optimal packing; most recent feature is rounding up SKU numbers according to sub-bundle values
</commit_message>
<xml_diff>
--- a/new_data/SO_Line_Items_12_Orders_Revised.xlsx
+++ b/new_data/SO_Line_Items_12_Orders_Revised.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\source\bundle-optimization-new\new_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\source\repos\Bundle_Optimization\new_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ECDA2C-CE40-4C14-B99B-82868A5398ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A6BF06-3A6E-458A-94A1-065C8E24F6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SKU_Quantities" sheetId="1" r:id="rId1"/>
@@ -387,26 +387,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,7 +463,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{113AECD6-0894-4C39-B958-FA7F0B6F746B}" name="Table1" displayName="Table1" ref="A1:H117" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:H117" xr:uid="{113AECD6-0894-4C39-B958-FA7F0B6F746B}"/>
+  <autoFilter ref="A1:H117" xr:uid="{113AECD6-0894-4C39-B958-FA7F0B6F746B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SO-1013210"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H117">
     <sortCondition ref="B1:B117"/>
   </sortState>
@@ -488,9 +488,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -528,9 +528,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -563,26 +563,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,26 +598,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -808,20 +774,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:D122"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -832,7 +799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -843,7 +810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -854,7 +821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -865,7 +832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -876,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -887,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -909,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -920,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -931,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -942,7 +909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -953,7 +920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -964,7 +931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -975,7 +942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -986,7 +953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -997,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1019,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1052,7 +1019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +1030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1041,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1107,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1118,7 +1085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
@@ -1140,7 +1107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1173,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
@@ -1184,7 +1151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -1206,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1217,7 +1184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -1250,7 +1217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
@@ -1261,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1239,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -1294,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>2</v>
       </c>
@@ -1316,7 +1283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -1327,7 +1294,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>3</v>
       </c>
@@ -1338,7 +1305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -1349,7 +1316,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
@@ -1360,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
@@ -1371,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -1382,7 +1349,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>2</v>
       </c>
@@ -1393,7 +1360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -1404,7 +1371,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>10</v>
       </c>
@@ -1415,7 +1382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
@@ -1437,7 +1404,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
@@ -1459,7 +1426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>12</v>
       </c>
@@ -1470,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>3</v>
       </c>
@@ -1481,7 +1448,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>8</v>
       </c>
@@ -1492,7 +1459,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
@@ -1503,7 +1470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -1514,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -1525,7 +1492,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
@@ -1547,7 +1514,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>10</v>
       </c>
@@ -1558,7 +1525,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1547,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -1591,7 +1558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -1602,7 +1569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -1613,7 +1580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>13</v>
       </c>
@@ -1624,7 +1591,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>2</v>
       </c>
@@ -1635,7 +1602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
@@ -1646,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>2</v>
       </c>
@@ -1657,7 +1624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>2</v>
       </c>
@@ -1668,7 +1635,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
@@ -1679,7 +1646,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
@@ -1690,7 +1657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -1701,194 +1668,194 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C81" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C82" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C83" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C84" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C85" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C86" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C87" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C88" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C89" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C90" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C91" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C92" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="4" t="s">
         <v>83</v>
       </c>
       <c r="C93" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C94" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C95" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>3</v>
       </c>
@@ -1899,7 +1866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>4</v>
       </c>
@@ -1921,7 +1888,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>4</v>
       </c>
@@ -1932,7 +1899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>3</v>
       </c>
@@ -1943,7 +1910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>13</v>
       </c>
@@ -1965,7 +1932,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>12</v>
       </c>
@@ -1976,7 +1943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
@@ -1987,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>2</v>
       </c>
@@ -1998,7 +1965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>2</v>
       </c>
@@ -2009,7 +1976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +1987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>3</v>
       </c>
@@ -2031,7 +1998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>13</v>
       </c>
@@ -2042,7 +2009,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>12</v>
       </c>
@@ -2053,7 +2020,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>11</v>
       </c>
@@ -2064,7 +2031,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>2</v>
       </c>
@@ -2075,7 +2042,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>2</v>
       </c>
@@ -2086,7 +2053,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
@@ -2097,7 +2064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
@@ -2108,7 +2075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>12</v>
       </c>
@@ -2119,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>13</v>
       </c>
@@ -2130,7 +2097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
@@ -2144,7 +2111,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>2</v>
       </c>
@@ -2155,7 +2122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>8</v>
       </c>
@@ -2168,6 +2135,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C122" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="SO-1013178"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C122">
       <sortCondition ref="B1:B122"/>
     </sortState>
@@ -2181,57 +2153,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B55D905-81B1-4C30-9105-ACE57A38A51C}">
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6">
+      <c r="D2">
         <v>6</v>
       </c>
       <c r="E2">
@@ -2247,15 +2218,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6">
+      <c r="D3">
         <v>14</v>
       </c>
       <c r="E3">
@@ -2271,15 +2241,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>6</v>
       </c>
       <c r="E4">
@@ -2295,15 +2264,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>6</v>
       </c>
       <c r="E5">
@@ -2319,15 +2287,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>1</v>
       </c>
       <c r="E6">
@@ -2343,15 +2310,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
@@ -2367,15 +2333,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>9</v>
       </c>
       <c r="E8">
@@ -2391,15 +2356,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>9</v>
       </c>
       <c r="E9">
@@ -2415,15 +2379,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
@@ -2439,15 +2402,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6">
+      <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
@@ -2463,15 +2425,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6">
+      <c r="D12">
         <v>13</v>
       </c>
       <c r="E12">
@@ -2487,15 +2448,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6">
+      <c r="D13">
         <v>7</v>
       </c>
       <c r="E13">
@@ -2511,15 +2471,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6">
+      <c r="D14">
         <v>6</v>
       </c>
       <c r="E14">
@@ -2535,15 +2494,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6">
+      <c r="D15">
         <v>20</v>
       </c>
       <c r="E15">
@@ -2559,15 +2517,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6">
+      <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
@@ -2583,15 +2540,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6">
+      <c r="D17">
         <v>4</v>
       </c>
       <c r="E17">
@@ -2607,15 +2563,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6">
+      <c r="D18">
         <v>3</v>
       </c>
       <c r="E18">
@@ -2631,15 +2586,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6">
+      <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
@@ -2655,15 +2609,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6">
+      <c r="D20">
         <v>3</v>
       </c>
       <c r="E20">
@@ -2679,15 +2632,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6">
+      <c r="D21">
         <v>37</v>
       </c>
       <c r="E21">
@@ -2703,15 +2655,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6">
+      <c r="D22">
         <v>3</v>
       </c>
       <c r="E22">
@@ -2727,15 +2678,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6">
+      <c r="D23">
         <v>12</v>
       </c>
       <c r="E23">
@@ -2751,15 +2701,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="7" t="s">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6">
+      <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
@@ -2775,15 +2724,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6">
+      <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
@@ -2799,15 +2747,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="7" t="s">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
@@ -2823,15 +2770,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6">
+      <c r="D27">
         <v>2</v>
       </c>
       <c r="E27">
@@ -2847,15 +2793,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6">
+      <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
@@ -2871,15 +2816,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6">
+      <c r="D29">
         <v>12</v>
       </c>
       <c r="E29">
@@ -2895,15 +2839,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6">
+      <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
@@ -2919,15 +2862,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6">
+      <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
@@ -2943,15 +2885,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B32" s="7" t="s">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6">
+      <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
@@ -2967,15 +2908,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6">
+      <c r="D33">
         <v>3</v>
       </c>
       <c r="E33">
@@ -2991,15 +2931,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6">
+      <c r="D34">
         <v>4</v>
       </c>
       <c r="E34">
@@ -3015,15 +2954,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6">
+      <c r="D35">
         <v>4</v>
       </c>
       <c r="E35">
@@ -3039,15 +2977,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6">
+      <c r="D36">
         <v>3</v>
       </c>
       <c r="E36">
@@ -3063,15 +3000,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="7" t="s">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6">
+      <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
@@ -3087,15 +3023,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="7" t="s">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6">
+      <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
@@ -3111,15 +3046,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="7" t="s">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6">
+      <c r="D39">
         <v>4</v>
       </c>
       <c r="E39">
@@ -3135,15 +3069,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="7" t="s">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6">
+      <c r="D40">
         <v>4</v>
       </c>
       <c r="E40">
@@ -3159,15 +3092,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6">
+      <c r="D41">
         <v>45</v>
       </c>
       <c r="E41">
@@ -3183,15 +3115,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6">
+      <c r="D42">
         <v>12</v>
       </c>
       <c r="E42">
@@ -3207,15 +3138,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6">
+      <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
@@ -3231,15 +3161,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="7" t="s">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6">
+      <c r="D44">
         <v>13</v>
       </c>
       <c r="E44">
@@ -3255,15 +3184,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6">
+      <c r="D45">
         <v>13</v>
       </c>
       <c r="E45">
@@ -3279,15 +3207,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6">
+      <c r="D46">
         <v>13</v>
       </c>
       <c r="E46">
@@ -3303,15 +3230,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6">
+      <c r="D47">
         <v>12</v>
       </c>
       <c r="E47">
@@ -3327,15 +3253,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6">
+      <c r="D48">
         <v>90</v>
       </c>
       <c r="E48">
@@ -3351,15 +3276,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6">
+      <c r="D49">
         <v>3</v>
       </c>
       <c r="E49">
@@ -3375,15 +3299,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6">
+      <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
@@ -3399,15 +3322,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="7" t="s">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6">
+      <c r="D51">
         <v>10</v>
       </c>
       <c r="E51">
@@ -3423,15 +3345,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="7" t="s">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6">
+      <c r="D52">
         <v>12</v>
       </c>
       <c r="E52">
@@ -3447,15 +3368,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B53" s="7" t="s">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6">
+      <c r="D53">
         <v>22</v>
       </c>
       <c r="E53">
@@ -3471,15 +3391,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6">
+      <c r="D54">
         <v>22</v>
       </c>
       <c r="E54">
@@ -3495,15 +3414,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6">
+      <c r="D55">
         <v>8</v>
       </c>
       <c r="E55">
@@ -3519,15 +3437,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6">
+      <c r="D56">
         <v>96</v>
       </c>
       <c r="E56">
@@ -3543,15 +3460,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="7" t="s">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6">
+      <c r="D57">
         <v>8</v>
       </c>
       <c r="E57">
@@ -3567,15 +3483,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6">
+      <c r="D58">
         <v>8</v>
       </c>
       <c r="E58">
@@ -3591,15 +3506,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>12</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6">
+      <c r="D59">
         <v>16</v>
       </c>
       <c r="E59">
@@ -3615,15 +3529,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6">
+      <c r="D60">
         <v>16</v>
       </c>
       <c r="E60">
@@ -3639,15 +3552,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6">
+      <c r="D61">
         <v>32</v>
       </c>
       <c r="E61">
@@ -3663,15 +3575,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>4</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6">
+      <c r="D62">
         <v>8</v>
       </c>
       <c r="E62">
@@ -3687,15 +3598,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B63" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6">
+      <c r="D63">
         <v>24</v>
       </c>
       <c r="E63">
@@ -3711,15 +3621,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6">
+      <c r="D64">
         <v>40</v>
       </c>
       <c r="E64">
@@ -3735,15 +3644,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6">
+      <c r="D65">
         <v>24</v>
       </c>
       <c r="E65">
@@ -3759,15 +3667,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6">
+      <c r="D66">
         <v>24</v>
       </c>
       <c r="E66">
@@ -3783,15 +3690,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6">
+      <c r="D67">
         <v>48</v>
       </c>
       <c r="E67">
@@ -3807,15 +3713,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6">
+      <c r="D68">
         <v>8</v>
       </c>
       <c r="E68">
@@ -3831,15 +3736,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6">
+      <c r="D69">
         <v>128</v>
       </c>
       <c r="E69">
@@ -3855,15 +3759,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>3</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6">
+      <c r="D70">
         <v>40</v>
       </c>
       <c r="E70">
@@ -3879,15 +3782,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>4</v>
       </c>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6">
+      <c r="D71">
         <v>48</v>
       </c>
       <c r="E71">
@@ -3903,15 +3805,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B72" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6">
+      <c r="D72">
         <v>8</v>
       </c>
       <c r="E72">
@@ -3927,15 +3828,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>13</v>
       </c>
-      <c r="B73" s="7" t="s">
+      <c r="B73" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6">
+      <c r="D73">
         <v>360</v>
       </c>
       <c r="E73">
@@ -3951,15 +3851,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="7" t="s">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6">
+      <c r="D74">
         <v>4</v>
       </c>
       <c r="E74">
@@ -3975,15 +3874,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="7" t="s">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6">
+      <c r="D75">
         <v>4</v>
       </c>
       <c r="E75">
@@ -3999,15 +3897,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="7" t="s">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6">
+      <c r="D76">
         <v>8</v>
       </c>
       <c r="E76">
@@ -4023,15 +3920,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" s="7" t="s">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="6"/>
-      <c r="D77" s="6">
+      <c r="D77">
         <v>96</v>
       </c>
       <c r="E77">
@@ -4047,15 +3943,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="6"/>
-      <c r="D78" s="6">
+      <c r="D78">
         <v>48</v>
       </c>
       <c r="E78">
@@ -4071,15 +3966,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6">
+      <c r="D79">
         <v>8</v>
       </c>
       <c r="E79">
@@ -4095,15 +3989,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="7" t="s">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6">
+      <c r="D80">
         <v>112</v>
       </c>
       <c r="E80">
@@ -4119,15 +4012,14 @@
         <v>7340.5999999999995</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="6" t="s">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>3</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="B81" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6">
+      <c r="D81">
         <v>2</v>
       </c>
       <c r="E81">
@@ -4143,15 +4035,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>3</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="B82" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6">
+      <c r="D82">
         <v>5</v>
       </c>
       <c r="E82">
@@ -4167,15 +4058,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C83" s="6"/>
-      <c r="D83" s="6">
+      <c r="D83">
         <v>1</v>
       </c>
       <c r="E83">
@@ -4191,15 +4081,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="6" t="s">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>5</v>
       </c>
-      <c r="B84" s="8" t="s">
+      <c r="B84" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6">
+      <c r="D84">
         <v>6</v>
       </c>
       <c r="E84">
@@ -4215,15 +4104,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>6</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6">
+      <c r="D85">
         <v>3</v>
       </c>
       <c r="E85">
@@ -4239,15 +4127,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6">
+      <c r="D86">
         <v>3</v>
       </c>
       <c r="E86">
@@ -4263,15 +4150,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="8" t="s">
+      <c r="B87" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6">
+      <c r="D87">
         <v>8</v>
       </c>
       <c r="E87">
@@ -4287,15 +4173,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="8" t="s">
+      <c r="B88" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6">
+      <c r="D88">
         <v>3</v>
       </c>
       <c r="E88">
@@ -4311,15 +4196,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>9</v>
       </c>
-      <c r="B89" s="8" t="s">
+      <c r="B89" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6">
+      <c r="D89">
         <v>7</v>
       </c>
       <c r="E89">
@@ -4335,15 +4219,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>10</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="B90" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6">
+      <c r="D90">
         <v>7</v>
       </c>
       <c r="E90">
@@ -4359,15 +4242,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="6" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>11</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="B91" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6">
+      <c r="D91">
         <v>2</v>
       </c>
       <c r="E91">
@@ -4383,15 +4265,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="8" t="s">
+      <c r="B92" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6">
+      <c r="D92">
         <v>2</v>
       </c>
       <c r="E92">
@@ -4407,15 +4288,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>13</v>
       </c>
-      <c r="B93" s="8" t="s">
+      <c r="B93" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="9">
+      <c r="D93">
         <v>4</v>
       </c>
       <c r="E93">
@@ -4431,15 +4311,14 @@
         <v>101.6</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="8" t="s">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6">
+      <c r="D94">
         <v>1</v>
       </c>
       <c r="E94">
@@ -4455,15 +4334,14 @@
         <v>152.39999999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="8" t="s">
+      <c r="B95" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6">
+      <c r="D95">
         <v>1</v>
       </c>
       <c r="E95">
@@ -4479,15 +4357,14 @@
         <v>152.39999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="8" t="s">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6">
+      <c r="D96">
         <v>1</v>
       </c>
       <c r="E96">
@@ -4503,15 +4380,14 @@
         <v>152.39999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>13</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="B97" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C97" s="6"/>
-      <c r="D97" s="9">
+      <c r="D97">
         <v>3</v>
       </c>
       <c r="E97">
@@ -4527,15 +4403,14 @@
         <v>152.39999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>3</v>
       </c>
-      <c r="B98" s="7" t="s">
+      <c r="B98" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6">
+      <c r="D98">
         <v>2</v>
       </c>
       <c r="E98">
@@ -4551,15 +4426,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>4</v>
       </c>
-      <c r="B99" s="7" t="s">
+      <c r="B99" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6">
+      <c r="D99">
         <v>10</v>
       </c>
       <c r="E99">
@@ -4575,15 +4449,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B100" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6">
+      <c r="D100">
         <v>10</v>
       </c>
       <c r="E100">
@@ -4599,15 +4472,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="6" t="s">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="7" t="s">
+      <c r="B101" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6">
+      <c r="D101">
         <v>8</v>
       </c>
       <c r="E101">
@@ -4623,15 +4495,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>3</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6">
+      <c r="D102">
         <v>2</v>
       </c>
       <c r="E102">
@@ -4647,15 +4518,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="6" t="s">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B103" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6">
+      <c r="D103">
         <v>1</v>
       </c>
       <c r="E103">
@@ -4671,15 +4541,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>13</v>
       </c>
-      <c r="B104" s="7" t="s">
+      <c r="B104" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6">
+      <c r="D104">
         <v>93</v>
       </c>
       <c r="E104">
@@ -4695,15 +4564,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>12</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6">
+      <c r="D105">
         <v>3</v>
       </c>
       <c r="E105">
@@ -4719,15 +4587,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>11</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6">
+      <c r="D106">
         <v>4</v>
       </c>
       <c r="E106">
@@ -4743,15 +4610,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="7" t="s">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6">
+      <c r="D107">
         <v>10</v>
       </c>
       <c r="E107">
@@ -4767,15 +4633,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="7" t="s">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6">
+      <c r="D108">
         <v>11</v>
       </c>
       <c r="E108">
@@ -4791,15 +4656,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="7" t="s">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6">
+      <c r="D109">
         <v>21</v>
       </c>
       <c r="E109">
@@ -4815,15 +4679,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>3</v>
       </c>
-      <c r="B110" s="7" t="s">
+      <c r="B110" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6">
+      <c r="D110">
         <v>12</v>
       </c>
       <c r="E110">
@@ -4839,15 +4702,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="6" t="s">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>13</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B111" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6">
+      <c r="D111">
         <v>113</v>
       </c>
       <c r="E111">
@@ -4863,15 +4725,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="6" t="s">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="7" t="s">
+      <c r="B112" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6">
+      <c r="D112">
         <v>5</v>
       </c>
       <c r="E112">
@@ -4887,15 +4748,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="6" t="s">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>11</v>
       </c>
-      <c r="B113" s="7" t="s">
+      <c r="B113" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6">
+      <c r="D113">
         <v>3</v>
       </c>
       <c r="E113">
@@ -4911,15 +4771,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="7" t="s">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6">
+      <c r="D114">
         <v>38</v>
       </c>
       <c r="E114">
@@ -4935,15 +4794,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="7" t="s">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6">
+      <c r="D115">
         <v>38</v>
       </c>
       <c r="E115">
@@ -4959,15 +4817,14 @@
         <v>3683</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="6" t="s">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>12</v>
       </c>
-      <c r="B116" s="7" t="s">
+      <c r="B116" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6">
+      <c r="D116">
         <v>1</v>
       </c>
       <c r="E116">
@@ -4983,15 +4840,14 @@
         <v>177.79999999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="6" t="s">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>13</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="B117" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6">
+      <c r="D117">
         <v>28</v>
       </c>
       <c r="E117">

</xml_diff>